<commit_message>
Implement excel parser with match points
</commit_message>
<xml_diff>
--- a/championship/tests/parsers/excel_ranking.xlsx
+++ b/championship/tests/parsers/excel_ranking.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t xml:space="preserve">RANK</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">MATCH_POINTS</t>
   </si>
@@ -146,71 +143,59 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="B1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="H9" activeCellId="0" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.68"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="B1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="C2" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>18</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>17</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="0" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>16</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>8</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>